<commit_message>
updates for import services
</commit_message>
<xml_diff>
--- a/relatedFiles/other files/EDITED service excel list - Copy.xlsx
+++ b/relatedFiles/other files/EDITED service excel list - Copy.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Dev\Laravel\_Developing_Phase_Project\Murarkey Single Vendor\Murarkey_single_vendor_ecommerce_with_vuexy_template\relatedFiles\other files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WEBROOT\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7B4299-B7FD-43AB-9D7C-181115C388CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="16980" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3516" yWindow="3516" windowWidth="16980" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="service excel list" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Unique sub sub cateogry" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'service excel list'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'service excel list'!$E:$E</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="0">'service excel list'!$J$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="196">
   <si>
     <t>Hair Cut</t>
   </si>
@@ -625,7 +626,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2867,6 +2868,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{381DB01D-C32E-4C56-B249-20873676A5EA}" type="pres">
       <dgm:prSet presAssocID="{E6D11840-871B-4461-AA2E-905FE378179A}" presName="root1" presStyleCnt="0"/>
@@ -2879,6 +2887,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{AA88D79D-77A2-4FA1-809E-218FECAFA084}" type="pres">
       <dgm:prSet presAssocID="{E6D11840-871B-4461-AA2E-905FE378179A}" presName="level2hierChild" presStyleCnt="0"/>
@@ -2887,10 +2902,24 @@
     <dgm:pt modelId="{05A2518B-1AD8-49B8-8A20-665744D76DE0}" type="pres">
       <dgm:prSet presAssocID="{01CC94C0-1719-4DA8-8EF4-C89122DE794E}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="4"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{76C328C3-790B-449A-B4EC-E26A5AB62DB3}" type="pres">
       <dgm:prSet presAssocID="{01CC94C0-1719-4DA8-8EF4-C89122DE794E}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="4"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{59C564CA-7204-41EB-A607-170D7366A2BE}" type="pres">
       <dgm:prSet presAssocID="{6B126DD3-344B-484C-A73A-96D648F39D6C}" presName="root2" presStyleCnt="0"/>
@@ -2903,6 +2932,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{C279E38C-E319-412D-BEBB-ACF07334F2AA}" type="pres">
       <dgm:prSet presAssocID="{6B126DD3-344B-484C-A73A-96D648F39D6C}" presName="level3hierChild" presStyleCnt="0"/>
@@ -2911,10 +2947,24 @@
     <dgm:pt modelId="{A310D4CC-9AD8-4FFD-86B5-B7A8B61EA796}" type="pres">
       <dgm:prSet presAssocID="{DF076996-6664-4169-94F7-1A778F527B39}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{659EB550-FD8A-41B0-B5F7-E25E40DAF562}" type="pres">
       <dgm:prSet presAssocID="{DF076996-6664-4169-94F7-1A778F527B39}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{913E0C16-E226-41E6-9C43-8D436724AEB4}" type="pres">
       <dgm:prSet presAssocID="{DF3457D7-1044-4841-B45A-F37310BE12B0}" presName="root2" presStyleCnt="0"/>
@@ -2927,6 +2977,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{AF640314-2ECE-4195-89E3-226E3A9976BD}" type="pres">
       <dgm:prSet presAssocID="{DF3457D7-1044-4841-B45A-F37310BE12B0}" presName="level3hierChild" presStyleCnt="0"/>
@@ -2935,10 +2992,24 @@
     <dgm:pt modelId="{C88BB0EC-34A0-4DD3-9B1D-2CFC1B7AD6BF}" type="pres">
       <dgm:prSet presAssocID="{B9333AA2-3BCC-4402-9FA4-B281D846CF27}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{73358667-9546-4460-9AFE-C527A4C98033}" type="pres">
       <dgm:prSet presAssocID="{B9333AA2-3BCC-4402-9FA4-B281D846CF27}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{6DA361E6-A6EA-4A6F-9488-6DCB36F3201C}" type="pres">
       <dgm:prSet presAssocID="{FF655F85-37A9-4E90-9EEB-F1432BEF706E}" presName="root2" presStyleCnt="0"/>
@@ -2951,6 +3022,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{FC59A8F9-3ABF-4C65-89A7-988BAB522800}" type="pres">
       <dgm:prSet presAssocID="{FF655F85-37A9-4E90-9EEB-F1432BEF706E}" presName="level3hierChild" presStyleCnt="0"/>
@@ -2959,10 +3037,24 @@
     <dgm:pt modelId="{5A1B14D3-2932-40E6-8277-B892B3A2C268}" type="pres">
       <dgm:prSet presAssocID="{2C2188DC-9466-4D6D-87B3-01C48C18E015}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{171B1A66-1ECD-4A64-BA46-F6C58D10E6A5}" type="pres">
       <dgm:prSet presAssocID="{2C2188DC-9466-4D6D-87B3-01C48C18E015}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{95048E7F-B26D-4257-A023-0F80DE34B799}" type="pres">
       <dgm:prSet presAssocID="{8C90B200-46F8-401B-B7A5-914D149C0AE4}" presName="root2" presStyleCnt="0"/>
@@ -2975,6 +3067,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{D278CE4E-7380-4E53-ACAB-302A8A391D96}" type="pres">
       <dgm:prSet presAssocID="{8C90B200-46F8-401B-B7A5-914D149C0AE4}" presName="level3hierChild" presStyleCnt="0"/>
@@ -2983,10 +3082,24 @@
     <dgm:pt modelId="{A5BF70C0-42B7-44FE-B0DC-09882320DFE8}" type="pres">
       <dgm:prSet presAssocID="{CC7EA531-4394-4DEB-900A-6CAE014C98B6}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{8AB96B72-E3AD-4FAF-9EAA-E7A920DC89D0}" type="pres">
       <dgm:prSet presAssocID="{CC7EA531-4394-4DEB-900A-6CAE014C98B6}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{18FC90F3-0B0D-4EC1-8CFD-83D41776A829}" type="pres">
       <dgm:prSet presAssocID="{E7B7B8BD-2EAA-4FA2-BC39-EDE5A74DB172}" presName="root2" presStyleCnt="0"/>
@@ -2999,6 +3112,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{9CD57FE8-B60B-4F3B-B68A-F12F4B8DB1B0}" type="pres">
       <dgm:prSet presAssocID="{E7B7B8BD-2EAA-4FA2-BC39-EDE5A74DB172}" presName="level3hierChild" presStyleCnt="0"/>
@@ -3007,10 +3127,24 @@
     <dgm:pt modelId="{D6AE0F14-8D03-4751-94EF-AE34C414DA2F}" type="pres">
       <dgm:prSet presAssocID="{89D1FB93-119C-4F70-B306-A1AF8BC304F3}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="4"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{06AC6E63-7B2C-4E8C-9F07-1FB541062587}" type="pres">
       <dgm:prSet presAssocID="{89D1FB93-119C-4F70-B306-A1AF8BC304F3}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="4"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{DFB4132E-1455-4F7C-976A-EDD24FF7E2A8}" type="pres">
       <dgm:prSet presAssocID="{69058FAB-016B-466B-A050-C1C21C940182}" presName="root2" presStyleCnt="0"/>
@@ -3023,6 +3157,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{B8D1B37F-8689-45B0-B2CF-438A5BC98706}" type="pres">
       <dgm:prSet presAssocID="{69058FAB-016B-466B-A050-C1C21C940182}" presName="level3hierChild" presStyleCnt="0"/>
@@ -3031,10 +3172,24 @@
     <dgm:pt modelId="{B730B3FD-843F-4BA2-AA8A-9C1C1F54F927}" type="pres">
       <dgm:prSet presAssocID="{F0DD7B8A-0054-441B-B9C2-D67D11219494}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="4" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{4F51D1A3-04DD-44C2-9512-E8B9C4880210}" type="pres">
       <dgm:prSet presAssocID="{F0DD7B8A-0054-441B-B9C2-D67D11219494}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="4" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{F7DA7F27-D855-4850-82DE-7D2E8C5BF87E}" type="pres">
       <dgm:prSet presAssocID="{B2997BBA-D8AD-4C0D-B208-E6519957635D}" presName="root2" presStyleCnt="0"/>
@@ -3047,6 +3202,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{E88858E0-19DF-4470-A055-AA20CF10EF01}" type="pres">
       <dgm:prSet presAssocID="{B2997BBA-D8AD-4C0D-B208-E6519957635D}" presName="level3hierChild" presStyleCnt="0"/>
@@ -3055,10 +3217,24 @@
     <dgm:pt modelId="{96C4F6F9-AD28-4608-BE1B-320E208828BA}" type="pres">
       <dgm:prSet presAssocID="{B0206A09-DBCE-44EA-BB7B-75CA2D2F2132}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="5" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{8AE93B7C-0DE2-4613-83A7-DAE2038F4EB3}" type="pres">
       <dgm:prSet presAssocID="{B0206A09-DBCE-44EA-BB7B-75CA2D2F2132}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="5" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{FC610C56-EFA2-40C3-9CAA-C1279091C6CF}" type="pres">
       <dgm:prSet presAssocID="{FC3BF431-AB1B-4781-AB91-1CAFFF4DA3F3}" presName="root2" presStyleCnt="0"/>
@@ -3071,6 +3247,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{BA412974-B5B8-4A70-A0C3-5017B296BC74}" type="pres">
       <dgm:prSet presAssocID="{FC3BF431-AB1B-4781-AB91-1CAFFF4DA3F3}" presName="level3hierChild" presStyleCnt="0"/>
@@ -3079,10 +3262,24 @@
     <dgm:pt modelId="{16169A5C-DE59-41AE-A0EB-E78F74755657}" type="pres">
       <dgm:prSet presAssocID="{95F10AA3-BF84-4C55-9FEE-C2A6778DCC23}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="4"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{A07A5A07-AD28-4A82-ADA3-A1CFED596CAC}" type="pres">
       <dgm:prSet presAssocID="{95F10AA3-BF84-4C55-9FEE-C2A6778DCC23}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="4"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{7E435F1A-B1DC-4978-8B8A-652D8E28B9E2}" type="pres">
       <dgm:prSet presAssocID="{83B849DD-1567-466E-B830-D7FBEABB7B7B}" presName="root2" presStyleCnt="0"/>
@@ -3095,6 +3292,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{C04D1362-AC83-48F0-80C5-834F3780EA5A}" type="pres">
       <dgm:prSet presAssocID="{83B849DD-1567-466E-B830-D7FBEABB7B7B}" presName="level3hierChild" presStyleCnt="0"/>
@@ -3103,10 +3307,24 @@
     <dgm:pt modelId="{4254C54C-F4AC-41F5-A3C9-625D0DF10069}" type="pres">
       <dgm:prSet presAssocID="{7C6C55D8-3CE0-4803-A2FE-0E18A7E2937D}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="6" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{154249D2-D116-4018-9D40-82ECA7B93510}" type="pres">
       <dgm:prSet presAssocID="{7C6C55D8-3CE0-4803-A2FE-0E18A7E2937D}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="6" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{CB292BB1-4BF7-4B8B-A5DA-5638288D0F32}" type="pres">
       <dgm:prSet presAssocID="{F7BC3D8C-9C61-4022-AC08-1190095E6220}" presName="root2" presStyleCnt="0"/>
@@ -3119,6 +3337,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{145D02C9-30E7-4660-BF1E-89BA824E88F1}" type="pres">
       <dgm:prSet presAssocID="{F7BC3D8C-9C61-4022-AC08-1190095E6220}" presName="level3hierChild" presStyleCnt="0"/>
@@ -3127,10 +3352,24 @@
     <dgm:pt modelId="{28AA50A7-F89D-49A4-B692-D689863D282B}" type="pres">
       <dgm:prSet presAssocID="{B1810F7F-300B-4FC1-8781-2D85C548DF8A}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="7" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{C591783A-195D-45BF-8DAC-86AEC03811EE}" type="pres">
       <dgm:prSet presAssocID="{B1810F7F-300B-4FC1-8781-2D85C548DF8A}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="7" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{A37DF041-A23A-4316-8E25-AF1C145068A1}" type="pres">
       <dgm:prSet presAssocID="{60F1B689-A05F-42BB-B986-749350EEB3DF}" presName="root2" presStyleCnt="0"/>
@@ -3143,6 +3382,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{89073CC5-2177-4C37-99C7-284E9710213F}" type="pres">
       <dgm:prSet presAssocID="{60F1B689-A05F-42BB-B986-749350EEB3DF}" presName="level3hierChild" presStyleCnt="0"/>
@@ -3151,10 +3397,24 @@
     <dgm:pt modelId="{67E00386-15B8-412F-9171-DF34B9D01F9A}" type="pres">
       <dgm:prSet presAssocID="{5C877E98-4F72-4008-A854-D7E76B8F99A8}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="8" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{544D1EDB-FE6B-4D6C-B1F6-B2F2EB7ABDCF}" type="pres">
       <dgm:prSet presAssocID="{5C877E98-4F72-4008-A854-D7E76B8F99A8}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="8" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{F38EA70E-E509-4E32-8E70-135A66BFF4BB}" type="pres">
       <dgm:prSet presAssocID="{8D8FD046-D864-4223-821E-1955630226F6}" presName="root2" presStyleCnt="0"/>
@@ -3167,6 +3427,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{29D46AD6-5BDC-472A-8C57-5067238C8A9B}" type="pres">
       <dgm:prSet presAssocID="{8D8FD046-D864-4223-821E-1955630226F6}" presName="level3hierChild" presStyleCnt="0"/>
@@ -3175,10 +3442,24 @@
     <dgm:pt modelId="{E009BEC9-02B3-4D9E-8DCC-15163BC39384}" type="pres">
       <dgm:prSet presAssocID="{7BE9D1C1-572E-49C8-BC63-5B4EF3B5A376}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="9" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{778B02FB-D1BD-4FC2-A491-D88F501DCC01}" type="pres">
       <dgm:prSet presAssocID="{7BE9D1C1-572E-49C8-BC63-5B4EF3B5A376}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="9" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{AE5FEB38-5BB8-42E1-837E-09FA9AE46AAD}" type="pres">
       <dgm:prSet presAssocID="{4485A2D2-9148-41E5-A3B1-6E6F35D8BF43}" presName="root2" presStyleCnt="0"/>
@@ -3191,6 +3472,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{75C5FBBC-5C6F-47CA-83A8-82C25C088785}" type="pres">
       <dgm:prSet presAssocID="{4485A2D2-9148-41E5-A3B1-6E6F35D8BF43}" presName="level3hierChild" presStyleCnt="0"/>
@@ -3199,10 +3487,24 @@
     <dgm:pt modelId="{E6977CD6-80D5-46D2-A8B4-33CF66DC7BD2}" type="pres">
       <dgm:prSet presAssocID="{7ADB3AFA-FB2E-449A-8FA1-1715ECD340C7}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="3" presStyleCnt="4"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{CF962479-FB1B-4B0A-BFE7-6892FE8FC40B}" type="pres">
       <dgm:prSet presAssocID="{7ADB3AFA-FB2E-449A-8FA1-1715ECD340C7}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="3" presStyleCnt="4"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{DAB5AD9B-A4ED-4F27-AC43-ABA84DC62E56}" type="pres">
       <dgm:prSet presAssocID="{605B26E4-A78B-481C-B8FC-9B6B5C784E43}" presName="root2" presStyleCnt="0"/>
@@ -3215,6 +3517,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{C740A465-86AF-468E-971B-1C806563994E}" type="pres">
       <dgm:prSet presAssocID="{605B26E4-A78B-481C-B8FC-9B6B5C784E43}" presName="level3hierChild" presStyleCnt="0"/>
@@ -3223,10 +3532,24 @@
     <dgm:pt modelId="{EF53EF41-4C69-4DAE-B69F-CBDC76EF5E5F}" type="pres">
       <dgm:prSet presAssocID="{E150C3AA-077F-40CC-BB7F-30BB81CB7151}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="10" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{D8D1A43C-7E25-4D47-98D4-7615D5B9C04B}" type="pres">
       <dgm:prSet presAssocID="{E150C3AA-077F-40CC-BB7F-30BB81CB7151}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="10" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{5DEBBC00-CD01-401A-95E1-889B914FB528}" type="pres">
       <dgm:prSet presAssocID="{0F952C35-842D-4109-8014-6D2E7F8C4D6B}" presName="root2" presStyleCnt="0"/>
@@ -3239,6 +3562,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{BB39FCDA-9BC4-48D6-A2C4-4632CA7C3BF1}" type="pres">
       <dgm:prSet presAssocID="{0F952C35-842D-4109-8014-6D2E7F8C4D6B}" presName="level3hierChild" presStyleCnt="0"/>
@@ -3247,10 +3577,24 @@
     <dgm:pt modelId="{BF6C354A-7990-44E5-A527-5EA2F1117AD8}" type="pres">
       <dgm:prSet presAssocID="{095FCC59-66C0-4192-8947-76487B777B8D}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="11" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{2F1CBDE8-656B-4018-83BD-B7541FC58CBC}" type="pres">
       <dgm:prSet presAssocID="{095FCC59-66C0-4192-8947-76487B777B8D}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="11" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{AF8049B8-F3B9-41FA-9C54-34B475D1FFE8}" type="pres">
       <dgm:prSet presAssocID="{DE06F1C4-6C8F-4AD0-9953-ADAFDAE04915}" presName="root2" presStyleCnt="0"/>
@@ -3263,6 +3607,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{F1415336-D21B-451B-B432-A25EC520522B}" type="pres">
       <dgm:prSet presAssocID="{DE06F1C4-6C8F-4AD0-9953-ADAFDAE04915}" presName="level3hierChild" presStyleCnt="0"/>
@@ -3271,10 +3622,24 @@
     <dgm:pt modelId="{8C6DE51C-0166-491A-8C9B-E28FCE8B0A5A}" type="pres">
       <dgm:prSet presAssocID="{EAC1DD83-76B8-439F-A49B-CAF8100FD997}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="12" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{9796A4D7-2609-4BFC-AFA8-A231A7AEE264}" type="pres">
       <dgm:prSet presAssocID="{EAC1DD83-76B8-439F-A49B-CAF8100FD997}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="12" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{768673C2-7942-4C40-8310-215CD9AB574A}" type="pres">
       <dgm:prSet presAssocID="{AB114299-C1BB-446E-B2B9-A34454524F8F}" presName="root2" presStyleCnt="0"/>
@@ -3287,6 +3652,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{A50D3EAD-F661-4745-809B-0A0EEE69D032}" type="pres">
       <dgm:prSet presAssocID="{AB114299-C1BB-446E-B2B9-A34454524F8F}" presName="level3hierChild" presStyleCnt="0"/>
@@ -3295,10 +3667,24 @@
     <dgm:pt modelId="{C37D8DE7-5AD2-4435-AE93-66BFD4E28671}" type="pres">
       <dgm:prSet presAssocID="{DC707BC5-E36D-423A-9224-A2E401015B11}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="13" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{7AF6027E-75E5-4F63-A080-2BDDF1D25ADF}" type="pres">
       <dgm:prSet presAssocID="{DC707BC5-E36D-423A-9224-A2E401015B11}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="13" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{1F093121-9A14-4649-96C3-AABFEF4876D2}" type="pres">
       <dgm:prSet presAssocID="{34C35C30-407D-496B-9882-98E4F29B14E8}" presName="root2" presStyleCnt="0"/>
@@ -3311,6 +3697,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{FDB80FF4-10F4-45E3-ACD5-8B070A338041}" type="pres">
       <dgm:prSet presAssocID="{34C35C30-407D-496B-9882-98E4F29B14E8}" presName="level3hierChild" presStyleCnt="0"/>
@@ -3319,10 +3712,24 @@
     <dgm:pt modelId="{52B7214D-6CEC-49F6-B00D-6F2E97508F19}" type="pres">
       <dgm:prSet presAssocID="{28AA64CB-2DE7-4E80-9E2E-9DACFF56FF0D}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="14" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{A48342EC-9DC8-429F-A225-614AFA551A36}" type="pres">
       <dgm:prSet presAssocID="{28AA64CB-2DE7-4E80-9E2E-9DACFF56FF0D}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="14" presStyleCnt="15"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{B22393E7-AB98-4377-90A3-9A40AB75FDFC}" type="pres">
       <dgm:prSet presAssocID="{77A6D86F-FF4E-4695-BCC5-E54F71481B00}" presName="root2" presStyleCnt="0"/>
@@ -3335,6 +3742,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{FAF9C34B-592B-4198-A462-A492FCE59115}" type="pres">
       <dgm:prSet presAssocID="{77A6D86F-FF4E-4695-BCC5-E54F71481B00}" presName="level3hierChild" presStyleCnt="0"/>
@@ -3342,85 +3756,85 @@
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
+    <dgm:cxn modelId="{16C9D57E-B671-465F-90A4-EA7F096EC2B3}" type="presOf" srcId="{B0206A09-DBCE-44EA-BB7B-75CA2D2F2132}" destId="{8AE93B7C-0DE2-4613-83A7-DAE2038F4EB3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{A5C91988-63BC-43E0-8FC7-4B5DFE639D4A}" type="presOf" srcId="{6B126DD3-344B-484C-A73A-96D648F39D6C}" destId="{B1D532EE-71F5-4CD3-82A3-0BD36A1F818A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{37002D05-1E05-4CB6-B0B9-2AE572C66BAC}" srcId="{605B26E4-A78B-481C-B8FC-9B6B5C784E43}" destId="{34C35C30-407D-496B-9882-98E4F29B14E8}" srcOrd="3" destOrd="0" parTransId="{DC707BC5-E36D-423A-9224-A2E401015B11}" sibTransId="{72BE30EE-B57A-4D10-B92C-31E081EF4BA6}"/>
+    <dgm:cxn modelId="{09AF3ECF-925D-409B-A97F-4574B1AE7E67}" srcId="{605B26E4-A78B-481C-B8FC-9B6B5C784E43}" destId="{0F952C35-842D-4109-8014-6D2E7F8C4D6B}" srcOrd="0" destOrd="0" parTransId="{E150C3AA-077F-40CC-BB7F-30BB81CB7151}" sibTransId="{7E59E3E2-5BEC-4ADB-B6CA-A52361FAA5AE}"/>
+    <dgm:cxn modelId="{FE07A84B-F6D6-4C06-9985-C7BE8CE7DE3D}" type="presOf" srcId="{B0206A09-DBCE-44EA-BB7B-75CA2D2F2132}" destId="{96C4F6F9-AD28-4608-BE1B-320E208828BA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{85A4F4C2-CA8E-4F89-9255-D642CDFB0F60}" srcId="{605B26E4-A78B-481C-B8FC-9B6B5C784E43}" destId="{AB114299-C1BB-446E-B2B9-A34454524F8F}" srcOrd="2" destOrd="0" parTransId="{EAC1DD83-76B8-439F-A49B-CAF8100FD997}" sibTransId="{5F34C50C-A07E-46B5-911C-BD3197F43FEE}"/>
+    <dgm:cxn modelId="{B217402E-53A0-457A-AA5E-88079414D640}" type="presOf" srcId="{B2997BBA-D8AD-4C0D-B208-E6519957635D}" destId="{C225698C-1C0F-409D-B23A-D817727C33E8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{08503D31-290C-4E44-B776-9B56647CFC4E}" srcId="{E6D11840-871B-4461-AA2E-905FE378179A}" destId="{69058FAB-016B-466B-A050-C1C21C940182}" srcOrd="1" destOrd="0" parTransId="{89D1FB93-119C-4F70-B306-A1AF8BC304F3}" sibTransId="{BB30C5C5-3CAD-49C2-8815-281726B33B83}"/>
+    <dgm:cxn modelId="{5AC0FAB5-D159-47EC-89B4-B8D128BD3ED4}" type="presOf" srcId="{CC7EA531-4394-4DEB-900A-6CAE014C98B6}" destId="{8AB96B72-E3AD-4FAF-9EAA-E7A920DC89D0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{BE7212B4-BA43-48C9-8CCA-FC2D479256A4}" type="presOf" srcId="{095FCC59-66C0-4192-8947-76487B777B8D}" destId="{2F1CBDE8-656B-4018-83BD-B7541FC58CBC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{8D0B13FD-85BE-443D-A6FD-F7C4EE8FD6DA}" type="presOf" srcId="{FF655F85-37A9-4E90-9EEB-F1432BEF706E}" destId="{470F9A0F-14DB-4B16-AEE9-FEC970E9719F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{0FAF60EF-7732-4C48-9D47-80D2C05A59A8}" type="presOf" srcId="{E7B7B8BD-2EAA-4FA2-BC39-EDE5A74DB172}" destId="{2AFE4E72-961A-458F-A969-D6E77AFBDDCF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{3B2030B5-6D6A-473F-9389-2BB9552851B6}" type="presOf" srcId="{5C877E98-4F72-4008-A854-D7E76B8F99A8}" destId="{544D1EDB-FE6B-4D6C-B1F6-B2F2EB7ABDCF}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{432BCCB4-27A9-4132-AA46-B329117069DE}" type="presOf" srcId="{2C2188DC-9466-4D6D-87B3-01C48C18E015}" destId="{171B1A66-1ECD-4A64-BA46-F6C58D10E6A5}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{442FCEB8-EFDC-436B-B3B2-E61C66D79F5B}" type="presOf" srcId="{DE06F1C4-6C8F-4AD0-9953-ADAFDAE04915}" destId="{0A2818E7-BD03-47CB-86F2-EC4E4E8D1A71}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{EA8F37F2-83C9-41F5-96D5-8EA236D0863E}" type="presOf" srcId="{60F1B689-A05F-42BB-B986-749350EEB3DF}" destId="{6644E2C8-28D9-451D-9014-053F918A4EE5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{6472AE75-85E7-49BF-AB8C-9F6CD2A8260F}" type="presOf" srcId="{DF076996-6664-4169-94F7-1A778F527B39}" destId="{A310D4CC-9AD8-4FFD-86B5-B7A8B61EA796}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{B24A4571-BC08-42F5-8C72-73807F36D0A8}" type="presOf" srcId="{F7BC3D8C-9C61-4022-AC08-1190095E6220}" destId="{CC75D048-BDB5-4CA5-883A-9160FA567D85}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{EED9E8D8-B61D-4A8D-B42B-2DCBF7086928}" srcId="{83B849DD-1567-466E-B830-D7FBEABB7B7B}" destId="{4485A2D2-9148-41E5-A3B1-6E6F35D8BF43}" srcOrd="3" destOrd="0" parTransId="{7BE9D1C1-572E-49C8-BC63-5B4EF3B5A376}" sibTransId="{BF06E601-C30A-4BF1-9A74-3538F99E90B0}"/>
+    <dgm:cxn modelId="{32CFC2F3-7FCF-49DC-9881-62BB6453A9F8}" type="presOf" srcId="{89D1FB93-119C-4F70-B306-A1AF8BC304F3}" destId="{06AC6E63-7B2C-4E8C-9F07-1FB541062587}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{3C8EFA9D-A074-4117-9A03-BCFCEFEE95CA}" srcId="{605B26E4-A78B-481C-B8FC-9B6B5C784E43}" destId="{DE06F1C4-6C8F-4AD0-9953-ADAFDAE04915}" srcOrd="1" destOrd="0" parTransId="{095FCC59-66C0-4192-8947-76487B777B8D}" sibTransId="{A245AA75-3490-47FC-8B44-F143DAB97ECD}"/>
+    <dgm:cxn modelId="{11DF377D-036D-435B-B750-D9E6AC0E8AD3}" type="presOf" srcId="{DF076996-6664-4169-94F7-1A778F527B39}" destId="{659EB550-FD8A-41B0-B5F7-E25E40DAF562}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{1CD25F66-BFB7-40A1-BA90-16E70E3ADF04}" type="presOf" srcId="{DC707BC5-E36D-423A-9224-A2E401015B11}" destId="{7AF6027E-75E5-4F63-A080-2BDDF1D25ADF}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{488B71B5-14F7-4FE5-9C3A-85D8E019BEFD}" type="presOf" srcId="{B9333AA2-3BCC-4402-9FA4-B281D846CF27}" destId="{73358667-9546-4460-9AFE-C527A4C98033}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{4311E1B1-FF51-4B9C-ADBE-DD52D0139672}" type="presOf" srcId="{8C90B200-46F8-401B-B7A5-914D149C0AE4}" destId="{EB54441C-A281-4B57-8519-B464FBDED4D6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{F2172594-16E3-47FB-9B86-02A863DB71E3}" type="presOf" srcId="{01CC94C0-1719-4DA8-8EF4-C89122DE794E}" destId="{05A2518B-1AD8-49B8-8A20-665744D76DE0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{3C3805EA-FC46-450D-BD11-F2A53B403B07}" type="presOf" srcId="{CC7EA531-4394-4DEB-900A-6CAE014C98B6}" destId="{A5BF70C0-42B7-44FE-B0DC-09882320DFE8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{35F2A6DA-886E-4782-A020-F54A5774A940}" type="presOf" srcId="{B9333AA2-3BCC-4402-9FA4-B281D846CF27}" destId="{C88BB0EC-34A0-4DD3-9B1D-2CFC1B7AD6BF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{44D25795-7A45-48AB-9CC7-E8F1A206B8B9}" type="presOf" srcId="{DC707BC5-E36D-423A-9224-A2E401015B11}" destId="{C37D8DE7-5AD2-4435-AE93-66BFD4E28671}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{9B5E174F-38AC-445D-BEE6-0E1AE2F81481}" type="presOf" srcId="{7ADB3AFA-FB2E-449A-8FA1-1715ECD340C7}" destId="{E6977CD6-80D5-46D2-A8B4-33CF66DC7BD2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{0D0CBCE6-B164-4106-910E-D71C3B7CF0E0}" type="presOf" srcId="{01CC94C0-1719-4DA8-8EF4-C89122DE794E}" destId="{76C328C3-790B-449A-B4EC-E26A5AB62DB3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{0AE9B1C7-0007-4DF4-BE3D-7737CA1BFA21}" type="presOf" srcId="{E6D11840-871B-4461-AA2E-905FE378179A}" destId="{4E6CD544-DFDA-4896-A772-61D5139C4444}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{44D2CFD3-345A-4F1C-981E-6A8B42FFFF07}" type="presOf" srcId="{AB114299-C1BB-446E-B2B9-A34454524F8F}" destId="{0518CC32-8AA5-42E4-BA6E-5C0EE4C31C9A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{358EECE5-0390-4170-BF2B-D511EDE25A55}" type="presOf" srcId="{77A6D86F-FF4E-4695-BCC5-E54F71481B00}" destId="{97FB63BE-77CE-42CC-A749-056C6B62B1F1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{2BE22692-8F05-487A-B43D-9E22FE1BB81D}" type="presOf" srcId="{89D1FB93-119C-4F70-B306-A1AF8BC304F3}" destId="{D6AE0F14-8D03-4751-94EF-AE34C414DA2F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{2DE87556-3101-4095-93C7-4BF645EF74F8}" type="presOf" srcId="{F0DD7B8A-0054-441B-B9C2-D67D11219494}" destId="{4F51D1A3-04DD-44C2-9512-E8B9C4880210}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{D1FB720B-D6F4-4AA9-8F44-A495C2757E2C}" type="presOf" srcId="{28AA64CB-2DE7-4E80-9E2E-9DACFF56FF0D}" destId="{A48342EC-9DC8-429F-A225-614AFA551A36}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{B15AF692-E4E0-46F1-ADEF-C4A96EDE885B}" srcId="{6B126DD3-344B-484C-A73A-96D648F39D6C}" destId="{8C90B200-46F8-401B-B7A5-914D149C0AE4}" srcOrd="2" destOrd="0" parTransId="{2C2188DC-9466-4D6D-87B3-01C48C18E015}" sibTransId="{D80DCFBF-476B-486B-87EC-D58D6146E5A8}"/>
+    <dgm:cxn modelId="{17EC7B53-EE1E-406F-BB07-32B4000F950E}" type="presOf" srcId="{34C35C30-407D-496B-9882-98E4F29B14E8}" destId="{DE8C2990-95EE-450C-B6AA-E85E0D3999B1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{4AC05277-44F9-4B0C-8CE2-FD302AE5918C}" type="presOf" srcId="{5C877E98-4F72-4008-A854-D7E76B8F99A8}" destId="{67E00386-15B8-412F-9171-DF34B9D01F9A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{74C218D6-E38B-4EF2-802B-361117B68120}" srcId="{E6D11840-871B-4461-AA2E-905FE378179A}" destId="{6B126DD3-344B-484C-A73A-96D648F39D6C}" srcOrd="0" destOrd="0" parTransId="{01CC94C0-1719-4DA8-8EF4-C89122DE794E}" sibTransId="{DA368B66-ECD2-4AE1-B91B-4C3BD7C04DB2}"/>
+    <dgm:cxn modelId="{9C0D7DB6-536B-4304-8C6B-2CEF1BA4E9B5}" type="presOf" srcId="{83B849DD-1567-466E-B830-D7FBEABB7B7B}" destId="{C0C02AD7-5AEE-4092-9A4F-3CEA3D4475F2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{99E9ED52-4B79-46A6-BBF6-D969CF7C5785}" type="presOf" srcId="{28AA64CB-2DE7-4E80-9E2E-9DACFF56FF0D}" destId="{52B7214D-6CEC-49F6-B00D-6F2E97508F19}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{79699550-3E85-45A0-8277-209D687D153C}" srcId="{83B849DD-1567-466E-B830-D7FBEABB7B7B}" destId="{8D8FD046-D864-4223-821E-1955630226F6}" srcOrd="2" destOrd="0" parTransId="{5C877E98-4F72-4008-A854-D7E76B8F99A8}" sibTransId="{51C24190-5406-4AA9-A7D0-4E64C07E93B6}"/>
+    <dgm:cxn modelId="{E14DB65B-E9CA-41C3-A31A-15946CD91D3D}" type="presOf" srcId="{FC3BF431-AB1B-4781-AB91-1CAFFF4DA3F3}" destId="{6BB08F02-10D0-4296-A276-9A8635A66B81}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{D24FFAC1-2C8A-4F89-BE96-FEAD27A68AA1}" srcId="{69058FAB-016B-466B-A050-C1C21C940182}" destId="{B2997BBA-D8AD-4C0D-B208-E6519957635D}" srcOrd="0" destOrd="0" parTransId="{F0DD7B8A-0054-441B-B9C2-D67D11219494}" sibTransId="{570FEEA9-4479-47CA-A194-2EF943F20482}"/>
+    <dgm:cxn modelId="{5A1DC6E7-26C3-4E2D-AB1C-F7297886CD52}" type="presOf" srcId="{95F10AA3-BF84-4C55-9FEE-C2A6778DCC23}" destId="{16169A5C-DE59-41AE-A0EB-E78F74755657}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{D08B275C-073F-448E-90C5-F7A2B6EE6416}" type="presOf" srcId="{7C6C55D8-3CE0-4803-A2FE-0E18A7E2937D}" destId="{154249D2-D116-4018-9D40-82ECA7B93510}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{1D1EDFAE-5BA1-453E-8136-D6F046EFD0E2}" type="presOf" srcId="{2C2188DC-9466-4D6D-87B3-01C48C18E015}" destId="{5A1B14D3-2932-40E6-8277-B892B3A2C268}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{F975CD0C-4715-405C-8636-E795B442B3F2}" type="presOf" srcId="{95F10AA3-BF84-4C55-9FEE-C2A6778DCC23}" destId="{A07A5A07-AD28-4A82-ADA3-A1CFED596CAC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{7326B69A-4749-4DD6-8E62-2D7587B98CD2}" srcId="{605B26E4-A78B-481C-B8FC-9B6B5C784E43}" destId="{77A6D86F-FF4E-4695-BCC5-E54F71481B00}" srcOrd="4" destOrd="0" parTransId="{28AA64CB-2DE7-4E80-9E2E-9DACFF56FF0D}" sibTransId="{AD5B5112-9FDD-49A0-BE03-A7EDCD2B9742}"/>
+    <dgm:cxn modelId="{AE996CEB-4B8A-452D-8936-5C9CB5FD95C8}" type="presOf" srcId="{7BE9D1C1-572E-49C8-BC63-5B4EF3B5A376}" destId="{778B02FB-D1BD-4FC2-A491-D88F501DCC01}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{62834E74-75E9-47A2-B4D2-EE3F37D1FC5B}" srcId="{83B849DD-1567-466E-B830-D7FBEABB7B7B}" destId="{F7BC3D8C-9C61-4022-AC08-1190095E6220}" srcOrd="0" destOrd="0" parTransId="{7C6C55D8-3CE0-4803-A2FE-0E18A7E2937D}" sibTransId="{DD60C7AD-F090-4358-BF41-152CE5702F00}"/>
+    <dgm:cxn modelId="{516D776B-5AD9-4E51-B20D-32400179C949}" srcId="{E6D11840-871B-4461-AA2E-905FE378179A}" destId="{83B849DD-1567-466E-B830-D7FBEABB7B7B}" srcOrd="2" destOrd="0" parTransId="{95F10AA3-BF84-4C55-9FEE-C2A6778DCC23}" sibTransId="{5FFA530B-32E3-4AAB-A73B-6BFDB76225DD}"/>
+    <dgm:cxn modelId="{58C6B130-C6AC-4F63-8095-D7AF98FFFB31}" type="presOf" srcId="{7BE9D1C1-572E-49C8-BC63-5B4EF3B5A376}" destId="{E009BEC9-02B3-4D9E-8DCC-15163BC39384}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{C672FF19-9F05-4621-BDBB-1410D9F4291B}" type="presOf" srcId="{69058FAB-016B-466B-A050-C1C21C940182}" destId="{762202AE-C40A-425F-B680-53BD2FE42362}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{9732015E-9D6F-4B16-9E0B-BC5FFD66AD92}" srcId="{6B126DD3-344B-484C-A73A-96D648F39D6C}" destId="{FF655F85-37A9-4E90-9EEB-F1432BEF706E}" srcOrd="1" destOrd="0" parTransId="{B9333AA2-3BCC-4402-9FA4-B281D846CF27}" sibTransId="{FEFA2F2C-3042-4F2B-8106-E99B74D2B632}"/>
+    <dgm:cxn modelId="{7A7CC728-1068-4348-85E6-609EFE54757E}" srcId="{69058FAB-016B-466B-A050-C1C21C940182}" destId="{FC3BF431-AB1B-4781-AB91-1CAFFF4DA3F3}" srcOrd="1" destOrd="0" parTransId="{B0206A09-DBCE-44EA-BB7B-75CA2D2F2132}" sibTransId="{A2C2097B-BDC8-4493-9F49-A32252ED0DF2}"/>
+    <dgm:cxn modelId="{350F10F1-9A41-49A4-9B33-4728EE0D37A7}" type="presOf" srcId="{F7CF5C9B-0058-428E-80A7-BBDD5DBBC35C}" destId="{C0ACF1DC-F97F-4C67-B6B9-BE9985EA1422}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{91685533-A888-4766-A99C-FDE7912F0518}" type="presOf" srcId="{4485A2D2-9148-41E5-A3B1-6E6F35D8BF43}" destId="{D8C62804-C33F-4313-8388-F2DD2AE99A3B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{EFE4B363-3B38-4B67-A48B-E839ECF8292C}" type="presOf" srcId="{DF3457D7-1044-4841-B45A-F37310BE12B0}" destId="{68195D3E-30A8-4DDA-A25F-13E53EA151D5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{19ABDC55-AA8F-4F81-94EE-BDCD860CE0AB}" type="presOf" srcId="{EAC1DD83-76B8-439F-A49B-CAF8100FD997}" destId="{8C6DE51C-0166-491A-8C9B-E28FCE8B0A5A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{D5C78088-0C43-4CFE-A2A5-6D8FB5C3090E}" srcId="{6B126DD3-344B-484C-A73A-96D648F39D6C}" destId="{E7B7B8BD-2EAA-4FA2-BC39-EDE5A74DB172}" srcOrd="3" destOrd="0" parTransId="{CC7EA531-4394-4DEB-900A-6CAE014C98B6}" sibTransId="{E08B3047-92D8-4EE7-9F4D-170912C6A44D}"/>
+    <dgm:cxn modelId="{01900F38-9C88-4CBE-BD48-C30B965BA981}" type="presOf" srcId="{B1810F7F-300B-4FC1-8781-2D85C548DF8A}" destId="{C591783A-195D-45BF-8DAC-86AEC03811EE}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{17989BFA-645B-49FA-91AA-7AFEC968643C}" srcId="{83B849DD-1567-466E-B830-D7FBEABB7B7B}" destId="{60F1B689-A05F-42BB-B986-749350EEB3DF}" srcOrd="1" destOrd="0" parTransId="{B1810F7F-300B-4FC1-8781-2D85C548DF8A}" sibTransId="{3B49177A-782B-4F58-9757-6460F89661B9}"/>
+    <dgm:cxn modelId="{E9885AC0-F0A6-4A0B-94D5-666ACB76221F}" type="presOf" srcId="{7C6C55D8-3CE0-4803-A2FE-0E18A7E2937D}" destId="{4254C54C-F4AC-41F5-A3C9-625D0DF10069}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{63615490-0D5E-4B13-B012-DDD5DEDBB863}" srcId="{E6D11840-871B-4461-AA2E-905FE378179A}" destId="{605B26E4-A78B-481C-B8FC-9B6B5C784E43}" srcOrd="3" destOrd="0" parTransId="{7ADB3AFA-FB2E-449A-8FA1-1715ECD340C7}" sibTransId="{8BA67377-4D74-4038-9CEF-AAEA9B533D10}"/>
+    <dgm:cxn modelId="{CD22CB78-98BE-4CB2-BA41-19CAE9D31A80}" type="presOf" srcId="{7ADB3AFA-FB2E-449A-8FA1-1715ECD340C7}" destId="{CF962479-FB1B-4B0A-BFE7-6892FE8FC40B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{AE0DB353-8924-4351-8EFA-903AAACC806C}" srcId="{6B126DD3-344B-484C-A73A-96D648F39D6C}" destId="{DF3457D7-1044-4841-B45A-F37310BE12B0}" srcOrd="0" destOrd="0" parTransId="{DF076996-6664-4169-94F7-1A778F527B39}" sibTransId="{72C64FDC-11B5-4A8C-B243-26FC7114F20F}"/>
+    <dgm:cxn modelId="{C8DDEECF-2D60-49F5-A997-13DB2948D03B}" type="presOf" srcId="{8D8FD046-D864-4223-821E-1955630226F6}" destId="{C7808D8B-3E58-4773-A3F9-09E70E321BA7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{82ACC419-4417-4799-A2E0-073650DEE5DD}" type="presOf" srcId="{605B26E4-A78B-481C-B8FC-9B6B5C784E43}" destId="{92A830D4-72B3-4753-B20E-9A400A383D91}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{C672FF19-9F05-4621-BDBB-1410D9F4291B}" type="presOf" srcId="{69058FAB-016B-466B-A050-C1C21C940182}" destId="{762202AE-C40A-425F-B680-53BD2FE42362}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{7A7CC728-1068-4348-85E6-609EFE54757E}" srcId="{69058FAB-016B-466B-A050-C1C21C940182}" destId="{FC3BF431-AB1B-4781-AB91-1CAFFF4DA3F3}" srcOrd="1" destOrd="0" parTransId="{B0206A09-DBCE-44EA-BB7B-75CA2D2F2132}" sibTransId="{A2C2097B-BDC8-4493-9F49-A32252ED0DF2}"/>
-    <dgm:cxn modelId="{B217402E-53A0-457A-AA5E-88079414D640}" type="presOf" srcId="{B2997BBA-D8AD-4C0D-B208-E6519957635D}" destId="{C225698C-1C0F-409D-B23A-D817727C33E8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{58C6B130-C6AC-4F63-8095-D7AF98FFFB31}" type="presOf" srcId="{7BE9D1C1-572E-49C8-BC63-5B4EF3B5A376}" destId="{E009BEC9-02B3-4D9E-8DCC-15163BC39384}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{08503D31-290C-4E44-B776-9B56647CFC4E}" srcId="{E6D11840-871B-4461-AA2E-905FE378179A}" destId="{69058FAB-016B-466B-A050-C1C21C940182}" srcOrd="1" destOrd="0" parTransId="{89D1FB93-119C-4F70-B306-A1AF8BC304F3}" sibTransId="{BB30C5C5-3CAD-49C2-8815-281726B33B83}"/>
-    <dgm:cxn modelId="{91685533-A888-4766-A99C-FDE7912F0518}" type="presOf" srcId="{4485A2D2-9148-41E5-A3B1-6E6F35D8BF43}" destId="{D8C62804-C33F-4313-8388-F2DD2AE99A3B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{01900F38-9C88-4CBE-BD48-C30B965BA981}" type="presOf" srcId="{B1810F7F-300B-4FC1-8781-2D85C548DF8A}" destId="{C591783A-195D-45BF-8DAC-86AEC03811EE}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{231CA7FA-71DA-4D39-BDE3-52010B29B90A}" type="presOf" srcId="{EAC1DD83-76B8-439F-A49B-CAF8100FD997}" destId="{9796A4D7-2609-4BFC-AFA8-A231A7AEE264}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{4BFF6994-F793-464A-8D41-EF78B57FB691}" type="presOf" srcId="{E150C3AA-077F-40CC-BB7F-30BB81CB7151}" destId="{EF53EF41-4C69-4DAE-B69F-CBDC76EF5E5F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{984743F6-0CFC-4822-A902-0A3202B802E1}" type="presOf" srcId="{F0DD7B8A-0054-441B-B9C2-D67D11219494}" destId="{B730B3FD-843F-4BA2-AA8A-9C1C1F54F927}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{C8F5767A-C118-47FB-A8D4-42BBED19A356}" type="presOf" srcId="{095FCC59-66C0-4192-8947-76487B777B8D}" destId="{BF6C354A-7990-44E5-A527-5EA2F1117AD8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{DB2DBA3F-E618-427D-BC5D-DBB9B05F811F}" type="presOf" srcId="{E150C3AA-077F-40CC-BB7F-30BB81CB7151}" destId="{D8D1A43C-7E25-4D47-98D4-7615D5B9C04B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{E14DB65B-E9CA-41C3-A31A-15946CD91D3D}" type="presOf" srcId="{FC3BF431-AB1B-4781-AB91-1CAFFF4DA3F3}" destId="{6BB08F02-10D0-4296-A276-9A8635A66B81}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{D08B275C-073F-448E-90C5-F7A2B6EE6416}" type="presOf" srcId="{7C6C55D8-3CE0-4803-A2FE-0E18A7E2937D}" destId="{154249D2-D116-4018-9D40-82ECA7B93510}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{9732015E-9D6F-4B16-9E0B-BC5FFD66AD92}" srcId="{6B126DD3-344B-484C-A73A-96D648F39D6C}" destId="{FF655F85-37A9-4E90-9EEB-F1432BEF706E}" srcOrd="1" destOrd="0" parTransId="{B9333AA2-3BCC-4402-9FA4-B281D846CF27}" sibTransId="{FEFA2F2C-3042-4F2B-8106-E99B74D2B632}"/>
-    <dgm:cxn modelId="{EFE4B363-3B38-4B67-A48B-E839ECF8292C}" type="presOf" srcId="{DF3457D7-1044-4841-B45A-F37310BE12B0}" destId="{68195D3E-30A8-4DDA-A25F-13E53EA151D5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{1CD25F66-BFB7-40A1-BA90-16E70E3ADF04}" type="presOf" srcId="{DC707BC5-E36D-423A-9224-A2E401015B11}" destId="{7AF6027E-75E5-4F63-A080-2BDDF1D25ADF}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{516D776B-5AD9-4E51-B20D-32400179C949}" srcId="{E6D11840-871B-4461-AA2E-905FE378179A}" destId="{83B849DD-1567-466E-B830-D7FBEABB7B7B}" srcOrd="2" destOrd="0" parTransId="{95F10AA3-BF84-4C55-9FEE-C2A6778DCC23}" sibTransId="{5FFA530B-32E3-4AAB-A73B-6BFDB76225DD}"/>
-    <dgm:cxn modelId="{FE07A84B-F6D6-4C06-9985-C7BE8CE7DE3D}" type="presOf" srcId="{B0206A09-DBCE-44EA-BB7B-75CA2D2F2132}" destId="{96C4F6F9-AD28-4608-BE1B-320E208828BA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{9B5E174F-38AC-445D-BEE6-0E1AE2F81481}" type="presOf" srcId="{7ADB3AFA-FB2E-449A-8FA1-1715ECD340C7}" destId="{E6977CD6-80D5-46D2-A8B4-33CF66DC7BD2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{79699550-3E85-45A0-8277-209D687D153C}" srcId="{83B849DD-1567-466E-B830-D7FBEABB7B7B}" destId="{8D8FD046-D864-4223-821E-1955630226F6}" srcOrd="2" destOrd="0" parTransId="{5C877E98-4F72-4008-A854-D7E76B8F99A8}" sibTransId="{51C24190-5406-4AA9-A7D0-4E64C07E93B6}"/>
-    <dgm:cxn modelId="{B24A4571-BC08-42F5-8C72-73807F36D0A8}" type="presOf" srcId="{F7BC3D8C-9C61-4022-AC08-1190095E6220}" destId="{CC75D048-BDB5-4CA5-883A-9160FA567D85}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{99E9ED52-4B79-46A6-BBF6-D969CF7C5785}" type="presOf" srcId="{28AA64CB-2DE7-4E80-9E2E-9DACFF56FF0D}" destId="{52B7214D-6CEC-49F6-B00D-6F2E97508F19}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{17EC7B53-EE1E-406F-BB07-32B4000F950E}" type="presOf" srcId="{34C35C30-407D-496B-9882-98E4F29B14E8}" destId="{DE8C2990-95EE-450C-B6AA-E85E0D3999B1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{AE0DB353-8924-4351-8EFA-903AAACC806C}" srcId="{6B126DD3-344B-484C-A73A-96D648F39D6C}" destId="{DF3457D7-1044-4841-B45A-F37310BE12B0}" srcOrd="0" destOrd="0" parTransId="{DF076996-6664-4169-94F7-1A778F527B39}" sibTransId="{72C64FDC-11B5-4A8C-B243-26FC7114F20F}"/>
-    <dgm:cxn modelId="{62834E74-75E9-47A2-B4D2-EE3F37D1FC5B}" srcId="{83B849DD-1567-466E-B830-D7FBEABB7B7B}" destId="{F7BC3D8C-9C61-4022-AC08-1190095E6220}" srcOrd="0" destOrd="0" parTransId="{7C6C55D8-3CE0-4803-A2FE-0E18A7E2937D}" sibTransId="{DD60C7AD-F090-4358-BF41-152CE5702F00}"/>
-    <dgm:cxn modelId="{6472AE75-85E7-49BF-AB8C-9F6CD2A8260F}" type="presOf" srcId="{DF076996-6664-4169-94F7-1A778F527B39}" destId="{A310D4CC-9AD8-4FFD-86B5-B7A8B61EA796}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{19ABDC55-AA8F-4F81-94EE-BDCD860CE0AB}" type="presOf" srcId="{EAC1DD83-76B8-439F-A49B-CAF8100FD997}" destId="{8C6DE51C-0166-491A-8C9B-E28FCE8B0A5A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{2DE87556-3101-4095-93C7-4BF645EF74F8}" type="presOf" srcId="{F0DD7B8A-0054-441B-B9C2-D67D11219494}" destId="{4F51D1A3-04DD-44C2-9512-E8B9C4880210}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{4AC05277-44F9-4B0C-8CE2-FD302AE5918C}" type="presOf" srcId="{5C877E98-4F72-4008-A854-D7E76B8F99A8}" destId="{67E00386-15B8-412F-9171-DF34B9D01F9A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{16D8E787-40FA-4FF2-BF85-1FDA961E25C3}" type="presOf" srcId="{B1810F7F-300B-4FC1-8781-2D85C548DF8A}" destId="{28AA50A7-F89D-49A4-B692-D689863D282B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{D9069658-6B6D-4EAC-8200-AD6941714AD8}" type="presOf" srcId="{0F952C35-842D-4109-8014-6D2E7F8C4D6B}" destId="{16F558F9-41FF-49C9-9B01-7823A77F160A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{CD22CB78-98BE-4CB2-BA41-19CAE9D31A80}" type="presOf" srcId="{7ADB3AFA-FB2E-449A-8FA1-1715ECD340C7}" destId="{CF962479-FB1B-4B0A-BFE7-6892FE8FC40B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{C8F5767A-C118-47FB-A8D4-42BBED19A356}" type="presOf" srcId="{095FCC59-66C0-4192-8947-76487B777B8D}" destId="{BF6C354A-7990-44E5-A527-5EA2F1117AD8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{11DF377D-036D-435B-B750-D9E6AC0E8AD3}" type="presOf" srcId="{DF076996-6664-4169-94F7-1A778F527B39}" destId="{659EB550-FD8A-41B0-B5F7-E25E40DAF562}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{16C9D57E-B671-465F-90A4-EA7F096EC2B3}" type="presOf" srcId="{B0206A09-DBCE-44EA-BB7B-75CA2D2F2132}" destId="{8AE93B7C-0DE2-4613-83A7-DAE2038F4EB3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{D276AA80-F22A-48AC-85F6-DD0A82302294}" srcId="{F7CF5C9B-0058-428E-80A7-BBDD5DBBC35C}" destId="{E6D11840-871B-4461-AA2E-905FE378179A}" srcOrd="0" destOrd="0" parTransId="{24050250-D2E2-4662-BDEC-58E74E1415E2}" sibTransId="{FACD7327-1F46-4EAB-833A-4B428EBD606B}"/>
-    <dgm:cxn modelId="{16D8E787-40FA-4FF2-BF85-1FDA961E25C3}" type="presOf" srcId="{B1810F7F-300B-4FC1-8781-2D85C548DF8A}" destId="{28AA50A7-F89D-49A4-B692-D689863D282B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{A5C91988-63BC-43E0-8FC7-4B5DFE639D4A}" type="presOf" srcId="{6B126DD3-344B-484C-A73A-96D648F39D6C}" destId="{B1D532EE-71F5-4CD3-82A3-0BD36A1F818A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{D5C78088-0C43-4CFE-A2A5-6D8FB5C3090E}" srcId="{6B126DD3-344B-484C-A73A-96D648F39D6C}" destId="{E7B7B8BD-2EAA-4FA2-BC39-EDE5A74DB172}" srcOrd="3" destOrd="0" parTransId="{CC7EA531-4394-4DEB-900A-6CAE014C98B6}" sibTransId="{E08B3047-92D8-4EE7-9F4D-170912C6A44D}"/>
-    <dgm:cxn modelId="{63615490-0D5E-4B13-B012-DDD5DEDBB863}" srcId="{E6D11840-871B-4461-AA2E-905FE378179A}" destId="{605B26E4-A78B-481C-B8FC-9B6B5C784E43}" srcOrd="3" destOrd="0" parTransId="{7ADB3AFA-FB2E-449A-8FA1-1715ECD340C7}" sibTransId="{8BA67377-4D74-4038-9CEF-AAEA9B533D10}"/>
-    <dgm:cxn modelId="{2BE22692-8F05-487A-B43D-9E22FE1BB81D}" type="presOf" srcId="{89D1FB93-119C-4F70-B306-A1AF8BC304F3}" destId="{D6AE0F14-8D03-4751-94EF-AE34C414DA2F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{B15AF692-E4E0-46F1-ADEF-C4A96EDE885B}" srcId="{6B126DD3-344B-484C-A73A-96D648F39D6C}" destId="{8C90B200-46F8-401B-B7A5-914D149C0AE4}" srcOrd="2" destOrd="0" parTransId="{2C2188DC-9466-4D6D-87B3-01C48C18E015}" sibTransId="{D80DCFBF-476B-486B-87EC-D58D6146E5A8}"/>
-    <dgm:cxn modelId="{F2172594-16E3-47FB-9B86-02A863DB71E3}" type="presOf" srcId="{01CC94C0-1719-4DA8-8EF4-C89122DE794E}" destId="{05A2518B-1AD8-49B8-8A20-665744D76DE0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{4BFF6994-F793-464A-8D41-EF78B57FB691}" type="presOf" srcId="{E150C3AA-077F-40CC-BB7F-30BB81CB7151}" destId="{EF53EF41-4C69-4DAE-B69F-CBDC76EF5E5F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{44D25795-7A45-48AB-9CC7-E8F1A206B8B9}" type="presOf" srcId="{DC707BC5-E36D-423A-9224-A2E401015B11}" destId="{C37D8DE7-5AD2-4435-AE93-66BFD4E28671}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{7326B69A-4749-4DD6-8E62-2D7587B98CD2}" srcId="{605B26E4-A78B-481C-B8FC-9B6B5C784E43}" destId="{77A6D86F-FF4E-4695-BCC5-E54F71481B00}" srcOrd="4" destOrd="0" parTransId="{28AA64CB-2DE7-4E80-9E2E-9DACFF56FF0D}" sibTransId="{AD5B5112-9FDD-49A0-BE03-A7EDCD2B9742}"/>
-    <dgm:cxn modelId="{3C8EFA9D-A074-4117-9A03-BCFCEFEE95CA}" srcId="{605B26E4-A78B-481C-B8FC-9B6B5C784E43}" destId="{DE06F1C4-6C8F-4AD0-9953-ADAFDAE04915}" srcOrd="1" destOrd="0" parTransId="{095FCC59-66C0-4192-8947-76487B777B8D}" sibTransId="{A245AA75-3490-47FC-8B44-F143DAB97ECD}"/>
-    <dgm:cxn modelId="{1D1EDFAE-5BA1-453E-8136-D6F046EFD0E2}" type="presOf" srcId="{2C2188DC-9466-4D6D-87B3-01C48C18E015}" destId="{5A1B14D3-2932-40E6-8277-B892B3A2C268}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{4311E1B1-FF51-4B9C-ADBE-DD52D0139672}" type="presOf" srcId="{8C90B200-46F8-401B-B7A5-914D149C0AE4}" destId="{EB54441C-A281-4B57-8519-B464FBDED4D6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{BE7212B4-BA43-48C9-8CCA-FC2D479256A4}" type="presOf" srcId="{095FCC59-66C0-4192-8947-76487B777B8D}" destId="{2F1CBDE8-656B-4018-83BD-B7541FC58CBC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{432BCCB4-27A9-4132-AA46-B329117069DE}" type="presOf" srcId="{2C2188DC-9466-4D6D-87B3-01C48C18E015}" destId="{171B1A66-1ECD-4A64-BA46-F6C58D10E6A5}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{3B2030B5-6D6A-473F-9389-2BB9552851B6}" type="presOf" srcId="{5C877E98-4F72-4008-A854-D7E76B8F99A8}" destId="{544D1EDB-FE6B-4D6C-B1F6-B2F2EB7ABDCF}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{488B71B5-14F7-4FE5-9C3A-85D8E019BEFD}" type="presOf" srcId="{B9333AA2-3BCC-4402-9FA4-B281D846CF27}" destId="{73358667-9546-4460-9AFE-C527A4C98033}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{5AC0FAB5-D159-47EC-89B4-B8D128BD3ED4}" type="presOf" srcId="{CC7EA531-4394-4DEB-900A-6CAE014C98B6}" destId="{8AB96B72-E3AD-4FAF-9EAA-E7A920DC89D0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{9C0D7DB6-536B-4304-8C6B-2CEF1BA4E9B5}" type="presOf" srcId="{83B849DD-1567-466E-B830-D7FBEABB7B7B}" destId="{C0C02AD7-5AEE-4092-9A4F-3CEA3D4475F2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{442FCEB8-EFDC-436B-B3B2-E61C66D79F5B}" type="presOf" srcId="{DE06F1C4-6C8F-4AD0-9953-ADAFDAE04915}" destId="{0A2818E7-BD03-47CB-86F2-EC4E4E8D1A71}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{E9885AC0-F0A6-4A0B-94D5-666ACB76221F}" type="presOf" srcId="{7C6C55D8-3CE0-4803-A2FE-0E18A7E2937D}" destId="{4254C54C-F4AC-41F5-A3C9-625D0DF10069}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{D24FFAC1-2C8A-4F89-BE96-FEAD27A68AA1}" srcId="{69058FAB-016B-466B-A050-C1C21C940182}" destId="{B2997BBA-D8AD-4C0D-B208-E6519957635D}" srcOrd="0" destOrd="0" parTransId="{F0DD7B8A-0054-441B-B9C2-D67D11219494}" sibTransId="{570FEEA9-4479-47CA-A194-2EF943F20482}"/>
-    <dgm:cxn modelId="{85A4F4C2-CA8E-4F89-9255-D642CDFB0F60}" srcId="{605B26E4-A78B-481C-B8FC-9B6B5C784E43}" destId="{AB114299-C1BB-446E-B2B9-A34454524F8F}" srcOrd="2" destOrd="0" parTransId="{EAC1DD83-76B8-439F-A49B-CAF8100FD997}" sibTransId="{5F34C50C-A07E-46B5-911C-BD3197F43FEE}"/>
-    <dgm:cxn modelId="{0AE9B1C7-0007-4DF4-BE3D-7737CA1BFA21}" type="presOf" srcId="{E6D11840-871B-4461-AA2E-905FE378179A}" destId="{4E6CD544-DFDA-4896-A772-61D5139C4444}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{09AF3ECF-925D-409B-A97F-4574B1AE7E67}" srcId="{605B26E4-A78B-481C-B8FC-9B6B5C784E43}" destId="{0F952C35-842D-4109-8014-6D2E7F8C4D6B}" srcOrd="0" destOrd="0" parTransId="{E150C3AA-077F-40CC-BB7F-30BB81CB7151}" sibTransId="{7E59E3E2-5BEC-4ADB-B6CA-A52361FAA5AE}"/>
-    <dgm:cxn modelId="{C8DDEECF-2D60-49F5-A997-13DB2948D03B}" type="presOf" srcId="{8D8FD046-D864-4223-821E-1955630226F6}" destId="{C7808D8B-3E58-4773-A3F9-09E70E321BA7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{44D2CFD3-345A-4F1C-981E-6A8B42FFFF07}" type="presOf" srcId="{AB114299-C1BB-446E-B2B9-A34454524F8F}" destId="{0518CC32-8AA5-42E4-BA6E-5C0EE4C31C9A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{74C218D6-E38B-4EF2-802B-361117B68120}" srcId="{E6D11840-871B-4461-AA2E-905FE378179A}" destId="{6B126DD3-344B-484C-A73A-96D648F39D6C}" srcOrd="0" destOrd="0" parTransId="{01CC94C0-1719-4DA8-8EF4-C89122DE794E}" sibTransId="{DA368B66-ECD2-4AE1-B91B-4C3BD7C04DB2}"/>
-    <dgm:cxn modelId="{EED9E8D8-B61D-4A8D-B42B-2DCBF7086928}" srcId="{83B849DD-1567-466E-B830-D7FBEABB7B7B}" destId="{4485A2D2-9148-41E5-A3B1-6E6F35D8BF43}" srcOrd="3" destOrd="0" parTransId="{7BE9D1C1-572E-49C8-BC63-5B4EF3B5A376}" sibTransId="{BF06E601-C30A-4BF1-9A74-3538F99E90B0}"/>
-    <dgm:cxn modelId="{35F2A6DA-886E-4782-A020-F54A5774A940}" type="presOf" srcId="{B9333AA2-3BCC-4402-9FA4-B281D846CF27}" destId="{C88BB0EC-34A0-4DD3-9B1D-2CFC1B7AD6BF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{358EECE5-0390-4170-BF2B-D511EDE25A55}" type="presOf" srcId="{77A6D86F-FF4E-4695-BCC5-E54F71481B00}" destId="{97FB63BE-77CE-42CC-A749-056C6B62B1F1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{0D0CBCE6-B164-4106-910E-D71C3B7CF0E0}" type="presOf" srcId="{01CC94C0-1719-4DA8-8EF4-C89122DE794E}" destId="{76C328C3-790B-449A-B4EC-E26A5AB62DB3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{5A1DC6E7-26C3-4E2D-AB1C-F7297886CD52}" type="presOf" srcId="{95F10AA3-BF84-4C55-9FEE-C2A6778DCC23}" destId="{16169A5C-DE59-41AE-A0EB-E78F74755657}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{3C3805EA-FC46-450D-BD11-F2A53B403B07}" type="presOf" srcId="{CC7EA531-4394-4DEB-900A-6CAE014C98B6}" destId="{A5BF70C0-42B7-44FE-B0DC-09882320DFE8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{AE996CEB-4B8A-452D-8936-5C9CB5FD95C8}" type="presOf" srcId="{7BE9D1C1-572E-49C8-BC63-5B4EF3B5A376}" destId="{778B02FB-D1BD-4FC2-A491-D88F501DCC01}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{0FAF60EF-7732-4C48-9D47-80D2C05A59A8}" type="presOf" srcId="{E7B7B8BD-2EAA-4FA2-BC39-EDE5A74DB172}" destId="{2AFE4E72-961A-458F-A969-D6E77AFBDDCF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{350F10F1-9A41-49A4-9B33-4728EE0D37A7}" type="presOf" srcId="{F7CF5C9B-0058-428E-80A7-BBDD5DBBC35C}" destId="{C0ACF1DC-F97F-4C67-B6B9-BE9985EA1422}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{EA8F37F2-83C9-41F5-96D5-8EA236D0863E}" type="presOf" srcId="{60F1B689-A05F-42BB-B986-749350EEB3DF}" destId="{6644E2C8-28D9-451D-9014-053F918A4EE5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{32CFC2F3-7FCF-49DC-9881-62BB6453A9F8}" type="presOf" srcId="{89D1FB93-119C-4F70-B306-A1AF8BC304F3}" destId="{06AC6E63-7B2C-4E8C-9F07-1FB541062587}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{984743F6-0CFC-4822-A902-0A3202B802E1}" type="presOf" srcId="{F0DD7B8A-0054-441B-B9C2-D67D11219494}" destId="{B730B3FD-843F-4BA2-AA8A-9C1C1F54F927}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{17989BFA-645B-49FA-91AA-7AFEC968643C}" srcId="{83B849DD-1567-466E-B830-D7FBEABB7B7B}" destId="{60F1B689-A05F-42BB-B986-749350EEB3DF}" srcOrd="1" destOrd="0" parTransId="{B1810F7F-300B-4FC1-8781-2D85C548DF8A}" sibTransId="{3B49177A-782B-4F58-9757-6460F89661B9}"/>
-    <dgm:cxn modelId="{231CA7FA-71DA-4D39-BDE3-52010B29B90A}" type="presOf" srcId="{EAC1DD83-76B8-439F-A49B-CAF8100FD997}" destId="{9796A4D7-2609-4BFC-AFA8-A231A7AEE264}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{8D0B13FD-85BE-443D-A6FD-F7C4EE8FD6DA}" type="presOf" srcId="{FF655F85-37A9-4E90-9EEB-F1432BEF706E}" destId="{470F9A0F-14DB-4B16-AEE9-FEC970E9719F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{AC608094-3E96-4F40-A84D-E7CE9B212969}" type="presParOf" srcId="{C0ACF1DC-F97F-4C67-B6B9-BE9985EA1422}" destId="{381DB01D-C32E-4C56-B249-20873676A5EA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{570F2C6A-A58F-42AD-BD53-3FF8A0568041}" type="presParOf" srcId="{381DB01D-C32E-4C56-B249-20873676A5EA}" destId="{4E6CD544-DFDA-4896-A772-61D5139C4444}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{2D5E6D56-D719-4DA9-9000-B1EC59205DFC}" type="presParOf" srcId="{381DB01D-C32E-4C56-B249-20873676A5EA}" destId="{AA88D79D-77A2-4FA1-809E-218FECAFA084}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
@@ -3545,8 +3959,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="652544" y="3940521"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="747784" y="3784860"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -3594,7 +4008,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3604,7 +4018,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -3613,8 +4026,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="667410" y="3955387"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="762063" y="3799139"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{05A2518B-1AD8-49B8-8A20-665744D76DE0}">
@@ -3624,8 +4037,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="16652881">
-          <a:off x="325099" y="2656840"/>
-          <a:ext cx="3091181" cy="10524"/>
+          <a:off x="433274" y="2551681"/>
+          <a:ext cx="2969071" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3639,7 +4052,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="3091181" y="5262"/>
+                <a:pt x="2969071" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3676,7 +4089,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="444500">
+          <a:pPr lvl="0" algn="ctr" defTabSz="444500">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3686,14 +4099,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="1000" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1793410" y="2584823"/>
-        <a:ext cx="154559" cy="154559"/>
+        <a:off x="1843583" y="2482716"/>
+        <a:ext cx="148453" cy="148453"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B1D532EE-71F5-4CD3-82A3-0BD36A1F818A}">
@@ -3703,8 +4115,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2073714" y="876124"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="2112814" y="841515"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -3752,7 +4164,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3762,7 +4174,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -3771,8 +4182,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2088580" y="890990"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="2127093" y="855794"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{A310D4CC-9AD8-4FFD-86B5-B7A8B61EA796}">
@@ -3782,8 +4193,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="17692822">
-          <a:off x="2809301" y="686871"/>
-          <a:ext cx="965116" cy="10524"/>
+          <a:off x="2819344" y="659530"/>
+          <a:ext cx="926991" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3797,7 +4208,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="965116" y="5262"/>
+                <a:pt x="926991" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3834,7 +4245,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3844,14 +4255,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3267731" y="668006"/>
-        <a:ext cx="48255" cy="48255"/>
+        <a:off x="3259665" y="641618"/>
+        <a:ext cx="46349" cy="46349"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{68195D3E-30A8-4DDA-A25F-13E53EA151D5}">
@@ -3861,8 +4271,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3494883" y="582"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="3477844" y="559"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -3910,7 +4320,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3920,7 +4330,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -3929,8 +4338,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3509749" y="15448"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="3492123" y="14838"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C88BB0EC-34A0-4DD3-9B1D-2CFC1B7AD6BF}">
@@ -3940,8 +4349,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="19457599">
-          <a:off x="3041834" y="978718"/>
-          <a:ext cx="500050" cy="10524"/>
+          <a:off x="3042691" y="939849"/>
+          <a:ext cx="480296" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3955,7 +4364,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="500050" y="5262"/>
+                <a:pt x="480296" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3992,7 +4401,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4002,14 +4411,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3279358" y="971480"/>
-        <a:ext cx="25002" cy="25002"/>
+        <a:off x="3270832" y="933104"/>
+        <a:ext cx="24014" cy="24014"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{470F9A0F-14DB-4B16-AEE9-FEC970E9719F}">
@@ -4019,8 +4427,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3494883" y="584277"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="3477844" y="561196"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -4068,7 +4476,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4078,7 +4486,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -4087,8 +4494,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3509749" y="599143"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="3492123" y="575475"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{5A1B14D3-2932-40E6-8277-B892B3A2C268}">
@@ -4098,8 +4505,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="2142401">
-          <a:off x="3041834" y="1270566"/>
-          <a:ext cx="500050" cy="10524"/>
+          <a:off x="3042691" y="1220167"/>
+          <a:ext cx="480296" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4113,7 +4520,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="500050" y="5262"/>
+                <a:pt x="480296" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4150,7 +4557,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4160,14 +4567,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3279358" y="1263327"/>
-        <a:ext cx="25002" cy="25002"/>
+        <a:off x="3270832" y="1213422"/>
+        <a:ext cx="24014" cy="24014"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{EB54441C-A281-4B57-8519-B464FBDED4D6}">
@@ -4177,8 +4583,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3494883" y="1167972"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="3477844" y="1121834"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -4226,7 +4632,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4236,7 +4642,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -4245,8 +4650,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3509749" y="1182838"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="3492123" y="1136113"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{A5BF70C0-42B7-44FE-B0DC-09882320DFE8}">
@@ -4256,8 +4661,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="3907178">
-          <a:off x="2809301" y="1562413"/>
-          <a:ext cx="965116" cy="10524"/>
+          <a:off x="2819344" y="1500486"/>
+          <a:ext cx="926991" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4271,7 +4676,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="965116" y="5262"/>
+                <a:pt x="926991" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4308,7 +4713,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4318,14 +4723,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3267731" y="1543548"/>
-        <a:ext cx="48255" cy="48255"/>
+        <a:off x="3259665" y="1482573"/>
+        <a:ext cx="46349" cy="46349"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{2AFE4E72-961A-458F-A969-D6E77AFBDDCF}">
@@ -4335,8 +4739,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3494883" y="1751666"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="3477844" y="1682471"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -4384,7 +4788,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4394,7 +4798,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -4403,8 +4806,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3509749" y="1766532"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="3492123" y="1696750"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{D6AE0F14-8D03-4751-94EF-AE34C414DA2F}">
@@ -4414,8 +4817,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="17230830">
-          <a:off x="1183364" y="3532382"/>
-          <a:ext cx="1374651" cy="10524"/>
+          <a:off x="1257635" y="3392636"/>
+          <a:ext cx="1320349" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4429,7 +4832,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="1374651" y="5262"/>
+                <a:pt x="1320349" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4466,7 +4869,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4476,14 +4879,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1836323" y="3503279"/>
-        <a:ext cx="68732" cy="68732"/>
+        <a:off x="1884801" y="3364890"/>
+        <a:ext cx="66017" cy="66017"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{762202AE-C40A-425F-B680-53BD2FE42362}">
@@ -4493,8 +4895,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2073714" y="2627208"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="2112814" y="2523427"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -4542,7 +4944,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4552,7 +4954,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -4561,8 +4962,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2088580" y="2642074"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="2127093" y="2537706"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B730B3FD-843F-4BA2-AA8A-9C1C1F54F927}">
@@ -4572,8 +4973,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="19457599">
-          <a:off x="3041834" y="2729802"/>
-          <a:ext cx="500050" cy="10524"/>
+          <a:off x="3042691" y="2621760"/>
+          <a:ext cx="480296" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4587,7 +4988,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="500050" y="5262"/>
+                <a:pt x="480296" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4624,7 +5025,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4634,14 +5035,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3279358" y="2722564"/>
-        <a:ext cx="25002" cy="25002"/>
+        <a:off x="3270832" y="2615015"/>
+        <a:ext cx="24014" cy="24014"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C225698C-1C0F-409D-B23A-D817727C33E8}">
@@ -4651,8 +5051,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3494883" y="2335361"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="3477844" y="2243108"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -4700,7 +5100,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4710,7 +5110,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -4719,8 +5118,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3509749" y="2350227"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="3492123" y="2257387"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{96C4F6F9-AD28-4608-BE1B-320E208828BA}">
@@ -4730,8 +5129,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="2142401">
-          <a:off x="3041834" y="3021650"/>
-          <a:ext cx="500050" cy="10524"/>
+          <a:off x="3042691" y="2902079"/>
+          <a:ext cx="480296" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4745,7 +5144,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="500050" y="5262"/>
+                <a:pt x="480296" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4782,7 +5181,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4792,14 +5191,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3279358" y="3014411"/>
-        <a:ext cx="25002" cy="25002"/>
+        <a:off x="3270832" y="2895334"/>
+        <a:ext cx="24014" cy="24014"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{6BB08F02-10D0-4296-A276-9A8635A66B81}">
@@ -4809,8 +5207,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3494883" y="2919055"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="3477844" y="2803745"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -4858,7 +5256,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4868,7 +5266,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -4877,8 +5274,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3509749" y="2933921"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="3492123" y="2818024"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{16169A5C-DE59-41AE-A0EB-E78F74755657}">
@@ -4888,8 +5285,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="2829178">
-          <a:off x="1572144" y="4407924"/>
-          <a:ext cx="597091" cy="10524"/>
+          <a:off x="1631057" y="4233592"/>
+          <a:ext cx="573505" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4903,7 +5300,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="597091" y="5262"/>
+                <a:pt x="573505" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4940,7 +5337,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4950,14 +5347,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1855762" y="4398260"/>
-        <a:ext cx="29854" cy="29854"/>
+        <a:off x="1903472" y="4224517"/>
+        <a:ext cx="28675" cy="28675"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C0C02AD7-5AEE-4092-9A4F-3CEA3D4475F2}">
@@ -4967,8 +5363,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2073714" y="4378292"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="2112814" y="4205338"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5016,7 +5412,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5026,7 +5422,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -5035,8 +5430,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2088580" y="4393158"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="2127093" y="4219617"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{4254C54C-F4AC-41F5-A3C9-625D0DF10069}">
@@ -5046,8 +5441,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="17692822">
-          <a:off x="2809301" y="4189039"/>
-          <a:ext cx="965116" cy="10524"/>
+          <a:off x="2819344" y="4023353"/>
+          <a:ext cx="926991" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5061,7 +5456,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="965116" y="5262"/>
+                <a:pt x="926991" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5098,7 +5493,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5108,14 +5503,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3267731" y="4170173"/>
-        <a:ext cx="48255" cy="48255"/>
+        <a:off x="3259665" y="4005441"/>
+        <a:ext cx="46349" cy="46349"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{CC75D048-BDB5-4CA5-883A-9160FA567D85}">
@@ -5125,8 +5519,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3494883" y="3502750"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="3477844" y="3364382"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5174,7 +5568,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5184,7 +5578,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -5193,8 +5586,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3509749" y="3517616"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="3492123" y="3378661"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{28AA50A7-F89D-49A4-B692-D689863D282B}">
@@ -5204,8 +5597,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="19457599">
-          <a:off x="3041834" y="4480886"/>
-          <a:ext cx="500050" cy="10524"/>
+          <a:off x="3042691" y="4303672"/>
+          <a:ext cx="480296" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5219,7 +5612,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="500050" y="5262"/>
+                <a:pt x="480296" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5256,7 +5649,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5266,14 +5659,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3279358" y="4473647"/>
-        <a:ext cx="25002" cy="25002"/>
+        <a:off x="3270832" y="4296927"/>
+        <a:ext cx="24014" cy="24014"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{6644E2C8-28D9-451D-9014-053F918A4EE5}">
@@ -5283,8 +5675,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3494883" y="4086445"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="3477844" y="3925020"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5332,7 +5724,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5342,7 +5734,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -5351,8 +5742,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3509749" y="4101311"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="3492123" y="3939299"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{67E00386-15B8-412F-9171-DF34B9D01F9A}">
@@ -5362,8 +5753,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="2142401">
-          <a:off x="3041834" y="4772734"/>
-          <a:ext cx="500050" cy="10524"/>
+          <a:off x="3042691" y="4583990"/>
+          <a:ext cx="480296" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5377,7 +5768,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="500050" y="5262"/>
+                <a:pt x="480296" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5414,7 +5805,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5424,14 +5815,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3279358" y="4765495"/>
-        <a:ext cx="25002" cy="25002"/>
+        <a:off x="3270832" y="4577245"/>
+        <a:ext cx="24014" cy="24014"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C7808D8B-3E58-4773-A3F9-09E70E321BA7}">
@@ -5441,8 +5831,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3494883" y="4670139"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="3477844" y="4485657"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5490,7 +5880,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5500,7 +5890,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -5509,8 +5898,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3509749" y="4685005"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="3492123" y="4499936"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E009BEC9-02B3-4D9E-8DCC-15163BC39384}">
@@ -5520,8 +5909,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="3907178">
-          <a:off x="2809301" y="5064581"/>
-          <a:ext cx="965116" cy="10524"/>
+          <a:off x="2819344" y="4864309"/>
+          <a:ext cx="926991" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5535,7 +5924,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="965116" y="5262"/>
+                <a:pt x="926991" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5572,7 +5961,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5582,14 +5971,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3267731" y="5045715"/>
-        <a:ext cx="48255" cy="48255"/>
+        <a:off x="3259665" y="4846397"/>
+        <a:ext cx="46349" cy="46349"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{D8C62804-C33F-4313-8388-F2DD2AE99A3B}">
@@ -5599,8 +5987,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3494883" y="5253834"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="3477844" y="5046294"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5648,7 +6036,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5658,7 +6046,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -5667,8 +6054,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3509749" y="5268700"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="3492123" y="5060573"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E6977CD6-80D5-46D2-A8B4-33CF66DC7BD2}">
@@ -5678,8 +6065,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="4947119">
-          <a:off x="325099" y="5721237"/>
-          <a:ext cx="3091181" cy="10524"/>
+          <a:off x="433274" y="5495026"/>
+          <a:ext cx="2969071" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5693,7 +6080,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="3091181" y="5262"/>
+                <a:pt x="2969071" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5730,7 +6117,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="444500">
+          <a:pPr lvl="0" algn="ctr" defTabSz="444500">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5740,14 +6127,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="1000" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1793410" y="5649220"/>
-        <a:ext cx="154559" cy="154559"/>
+        <a:off x="1843583" y="5426062"/>
+        <a:ext cx="148453" cy="148453"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{92A830D4-72B3-4753-B20E-9A400A383D91}">
@@ -5757,8 +6143,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2073714" y="7004918"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="2112814" y="6728206"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5806,7 +6192,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5816,7 +6202,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -5825,8 +6210,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2088580" y="7019784"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="2127093" y="6742485"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{EF53EF41-4C69-4DAE-B69F-CBDC76EF5E5F}">
@@ -5836,8 +6221,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="17350740">
-          <a:off x="2673864" y="6669741"/>
-          <a:ext cx="1235990" cy="10524"/>
+          <a:off x="2689256" y="6406061"/>
+          <a:ext cx="1187165" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5851,7 +6236,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="1235990" y="5262"/>
+                <a:pt x="1187165" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5888,7 +6273,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5898,14 +6283,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3260960" y="6644104"/>
-        <a:ext cx="61799" cy="61799"/>
+        <a:off x="3253160" y="6381645"/>
+        <a:ext cx="59358" cy="59358"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{16F558F9-41FF-49C9-9B01-7823A77F160A}">
@@ -5915,8 +6299,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3494883" y="5837529"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="3477844" y="5606931"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5964,7 +6348,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5974,7 +6358,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -5983,8 +6366,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3509749" y="5852395"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="3492123" y="5621210"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{BF6C354A-7990-44E5-A527-5EA2F1117AD8}">
@@ -5994,8 +6377,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="18289469">
-          <a:off x="2936340" y="6961588"/>
-          <a:ext cx="711037" cy="10524"/>
+          <a:off x="2941364" y="6686380"/>
+          <a:ext cx="682949" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6009,7 +6392,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="711037" y="5262"/>
+                <a:pt x="682949" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6046,7 +6429,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6056,14 +6439,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3274083" y="6949075"/>
-        <a:ext cx="35551" cy="35551"/>
+        <a:off x="3265766" y="6674569"/>
+        <a:ext cx="34147" cy="34147"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{0A2818E7-BD03-47CB-86F2-EC4E4E8D1A71}">
@@ -6073,8 +6455,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3494883" y="6421223"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="3477844" y="6167569"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6122,7 +6504,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6132,7 +6514,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -6141,8 +6522,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3509749" y="6436089"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="3492123" y="6181848"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{8C6DE51C-0166-491A-8C9B-E28FCE8B0A5A}">
@@ -6152,8 +6533,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3088835" y="7253436"/>
-          <a:ext cx="406048" cy="10524"/>
+          <a:off x="3087835" y="6966699"/>
+          <a:ext cx="390008" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6167,7 +6548,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="406048" y="5262"/>
+                <a:pt x="390008" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6204,7 +6585,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6214,14 +6595,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3281708" y="7248547"/>
-        <a:ext cx="20302" cy="20302"/>
+        <a:off x="3273089" y="6962211"/>
+        <a:ext cx="19500" cy="19500"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{0518CC32-8AA5-42E4-BA6E-5C0EE4C31C9A}">
@@ -6231,8 +6611,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3494883" y="7004918"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="3477844" y="6728206"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6280,7 +6660,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6290,7 +6670,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -6299,8 +6678,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3509749" y="7019784"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="3492123" y="6742485"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C37D8DE7-5AD2-4435-AE93-66BFD4E28671}">
@@ -6310,8 +6689,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="3310531">
-          <a:off x="2936340" y="7545283"/>
-          <a:ext cx="711037" cy="10524"/>
+          <a:off x="2941364" y="7247017"/>
+          <a:ext cx="682949" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6325,7 +6704,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="711037" y="5262"/>
+                <a:pt x="682949" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6362,7 +6741,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6372,14 +6751,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3274083" y="7532770"/>
-        <a:ext cx="35551" cy="35551"/>
+        <a:off x="3265766" y="7235206"/>
+        <a:ext cx="34147" cy="34147"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{DE8C2990-95EE-450C-B6AA-E85E0D3999B1}">
@@ -6389,8 +6767,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3494883" y="7588613"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="3477844" y="7288843"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6438,7 +6816,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6448,7 +6826,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -6457,8 +6834,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3509749" y="7603479"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="3492123" y="7303122"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{52B7214D-6CEC-49F6-B00D-6F2E97508F19}">
@@ -6468,8 +6845,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="4249260">
-          <a:off x="2673864" y="7837130"/>
-          <a:ext cx="1235990" cy="10524"/>
+          <a:off x="2689256" y="7527336"/>
+          <a:ext cx="1187165" cy="10524"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6483,7 +6860,7 @@
                 <a:pt x="0" y="5262"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="1235990" y="5262"/>
+                <a:pt x="1187165" y="5262"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6520,7 +6897,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6530,14 +6907,13 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-IN" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3260960" y="7811493"/>
-        <a:ext cx="61799" cy="61799"/>
+        <a:off x="3253160" y="7502919"/>
+        <a:ext cx="59358" cy="59358"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{97FB63BE-77CE-42CC-A749-056C6B62B1F1}">
@@ -6547,8 +6923,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3494883" y="8172307"/>
-          <a:ext cx="1015121" cy="507560"/>
+          <a:off x="3477844" y="7849480"/>
+          <a:ext cx="975021" cy="487510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6596,7 +6972,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="533400">
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6606,7 +6982,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-IN" sz="1200" kern="1200"/>
@@ -6615,8 +6990,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3509749" y="8187173"/>
-        <a:ext cx="985389" cy="477828"/>
+        <a:off x="3492123" y="7863759"/>
+        <a:ext cx="946463" cy="458952"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -8094,23 +8469,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -8146,23 +8504,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8338,24 +8679,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F109"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="1" max="1" width="41.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" customWidth="1"/>
+    <col min="6" max="6" width="51.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>136</v>
       </c>
@@ -8374,8 +8717,14 @@
       <c r="F1" s="9" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I1" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8394,8 +8743,12 @@
       <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I2" s="11"/>
+      <c r="J2" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -8414,8 +8767,12 @@
       <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I3" s="11"/>
+      <c r="J3" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -8434,8 +8791,12 @@
       <c r="F4" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I4" s="11"/>
+      <c r="J4" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -8454,8 +8815,12 @@
       <c r="F5" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I5" s="11"/>
+      <c r="J5" s="14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -8474,8 +8839,12 @@
       <c r="F6" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I6" s="11"/>
+      <c r="J6" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -8494,8 +8863,12 @@
       <c r="F7" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I7" s="11"/>
+      <c r="J7" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -8514,8 +8887,12 @@
       <c r="F8" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I8" s="11"/>
+      <c r="J8" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -8534,8 +8911,12 @@
       <c r="F9" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I9" s="11"/>
+      <c r="J9" s="14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -8554,8 +8935,12 @@
       <c r="F10" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I10" s="11"/>
+      <c r="J10" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -8574,8 +8959,12 @@
       <c r="F11" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I11" s="11"/>
+      <c r="J11" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -8594,8 +8983,12 @@
       <c r="F12" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I12" s="11"/>
+      <c r="J12" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -8614,8 +9007,12 @@
       <c r="F13" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I13" s="11"/>
+      <c r="J13" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -8634,8 +9031,12 @@
       <c r="F14" s="3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I14" s="11"/>
+      <c r="J14" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -8654,8 +9055,12 @@
       <c r="F15" s="3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I15" s="11"/>
+      <c r="J15" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -8674,8 +9079,12 @@
       <c r="F16" s="3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I16" s="11"/>
+      <c r="J16" s="14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -8694,8 +9103,12 @@
       <c r="F17" s="3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I17" s="12"/>
+      <c r="J17" s="14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -8714,8 +9127,11 @@
       <c r="F18" s="3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J18" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -8734,8 +9150,11 @@
       <c r="F19" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J19" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -8754,8 +9173,11 @@
       <c r="F20" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J20" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -8774,8 +9196,11 @@
       <c r="F21" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J21" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -8794,8 +9219,11 @@
       <c r="F22" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J22" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
@@ -8814,8 +9242,11 @@
       <c r="F23" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J23" s="14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -8834,8 +9265,11 @@
       <c r="F24" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J24" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -8854,8 +9288,11 @@
       <c r="F25" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J25" s="14" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
@@ -8874,8 +9311,11 @@
       <c r="F26" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J26" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
@@ -8894,8 +9334,11 @@
       <c r="F27" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J27" s="14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
@@ -8914,8 +9357,11 @@
       <c r="F28" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J28" s="14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
@@ -8934,8 +9380,11 @@
       <c r="F29" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J29" s="14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
@@ -8954,8 +9403,11 @@
       <c r="F30" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J30" s="14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
@@ -8974,8 +9426,11 @@
       <c r="F31" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J31" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
@@ -8994,8 +9449,11 @@
       <c r="F32" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J32" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -9014,8 +9472,11 @@
       <c r="F33" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J33" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -9034,8 +9495,11 @@
       <c r="F34" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J34" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -9054,8 +9518,11 @@
       <c r="F35" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J35" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -9074,8 +9541,11 @@
       <c r="F36" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J36" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>42</v>
       </c>
@@ -9094,8 +9564,11 @@
       <c r="F37" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J37" s="14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
@@ -9114,8 +9587,11 @@
       <c r="F38" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J38" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
@@ -9134,8 +9610,11 @@
       <c r="F39" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J39" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>45</v>
       </c>
@@ -9154,8 +9633,11 @@
       <c r="F40" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J40" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>47</v>
       </c>
@@ -9174,8 +9656,11 @@
       <c r="F41" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J41" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>48</v>
       </c>
@@ -9194,8 +9679,11 @@
       <c r="F42" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J42" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>49</v>
       </c>
@@ -9214,8 +9702,11 @@
       <c r="F43" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J43" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>50</v>
       </c>
@@ -9234,8 +9725,11 @@
       <c r="F44" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J44" s="14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>52</v>
       </c>
@@ -9254,8 +9748,11 @@
       <c r="F45" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J45" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
@@ -9274,8 +9771,11 @@
       <c r="F46" s="3" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J46" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>54</v>
       </c>
@@ -9294,8 +9794,11 @@
       <c r="F47" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J47" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>56</v>
       </c>
@@ -9314,8 +9817,11 @@
       <c r="F48" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J48" s="14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>57</v>
       </c>
@@ -9334,8 +9840,11 @@
       <c r="F49" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J49" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>58</v>
       </c>
@@ -9354,8 +9863,11 @@
       <c r="F50" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J50" s="14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>59</v>
       </c>
@@ -9374,8 +9886,11 @@
       <c r="F51" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J51" s="14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>60</v>
       </c>
@@ -9394,8 +9909,11 @@
       <c r="F52" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J52" s="14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>62</v>
       </c>
@@ -9414,8 +9932,11 @@
       <c r="F53" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J53" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>63</v>
       </c>
@@ -9434,8 +9955,11 @@
       <c r="F54" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J54" s="14" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>64</v>
       </c>
@@ -9454,8 +9978,11 @@
       <c r="F55" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J55" s="14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>65</v>
       </c>
@@ -9474,8 +10001,11 @@
       <c r="F56" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J56" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>66</v>
       </c>
@@ -9494,8 +10024,11 @@
       <c r="F57" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J57" s="14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>67</v>
       </c>
@@ -9514,8 +10047,11 @@
       <c r="F58" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J58" s="14" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>68</v>
       </c>
@@ -9534,8 +10070,11 @@
       <c r="F59" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J59" s="14" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>69</v>
       </c>
@@ -9554,8 +10093,11 @@
       <c r="F60" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J60" s="14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>70</v>
       </c>
@@ -9574,8 +10116,11 @@
       <c r="F61" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J61" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>71</v>
       </c>
@@ -9594,8 +10139,11 @@
       <c r="F62" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J62" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>73</v>
       </c>
@@ -9614,8 +10162,11 @@
       <c r="F63" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J63" s="14" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>75</v>
       </c>
@@ -9634,8 +10185,11 @@
       <c r="F64" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J64" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>76</v>
       </c>
@@ -9654,8 +10208,11 @@
       <c r="F65" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J65" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>77</v>
       </c>
@@ -9674,8 +10231,11 @@
       <c r="F66" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J66" s="14" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>79</v>
       </c>
@@ -9694,8 +10254,11 @@
       <c r="F67" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J67" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>157</v>
       </c>
@@ -9714,8 +10277,11 @@
       <c r="F68" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J68" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>81</v>
       </c>
@@ -9735,7 +10301,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>83</v>
       </c>
@@ -9755,7 +10321,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>84</v>
       </c>
@@ -9775,7 +10341,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>85</v>
       </c>
@@ -9795,7 +10361,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>87</v>
       </c>
@@ -9815,7 +10381,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>88</v>
       </c>
@@ -9835,7 +10401,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>89</v>
       </c>
@@ -9855,7 +10421,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>91</v>
       </c>
@@ -9875,7 +10441,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>93</v>
       </c>
@@ -9895,7 +10461,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>94</v>
       </c>
@@ -9915,7 +10481,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>156</v>
       </c>
@@ -9935,7 +10501,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>96</v>
       </c>
@@ -9955,7 +10521,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>97</v>
       </c>
@@ -9975,7 +10541,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>99</v>
       </c>
@@ -9995,7 +10561,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>100</v>
       </c>
@@ -10015,7 +10581,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>101</v>
       </c>
@@ -10035,7 +10601,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>102</v>
       </c>
@@ -10055,7 +10621,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>104</v>
       </c>
@@ -10075,7 +10641,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>105</v>
       </c>
@@ -10095,7 +10661,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>106</v>
       </c>
@@ -10115,7 +10681,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>108</v>
       </c>
@@ -10135,7 +10701,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>109</v>
       </c>
@@ -10155,7 +10721,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>110</v>
       </c>
@@ -10175,7 +10741,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>111</v>
       </c>
@@ -10195,7 +10761,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>113</v>
       </c>
@@ -10215,7 +10781,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>114</v>
       </c>
@@ -10235,7 +10801,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>115</v>
       </c>
@@ -10255,7 +10821,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>117</v>
       </c>
@@ -10275,7 +10841,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>118</v>
       </c>
@@ -10295,7 +10861,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>119</v>
       </c>
@@ -10315,7 +10881,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>120</v>
       </c>
@@ -10335,7 +10901,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>122</v>
       </c>
@@ -10355,7 +10921,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>124</v>
       </c>
@@ -10375,7 +10941,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>125</v>
       </c>
@@ -10395,7 +10961,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>126</v>
       </c>
@@ -10415,7 +10981,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>127</v>
       </c>
@@ -10435,7 +11001,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>128</v>
       </c>
@@ -10455,7 +11021,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>130</v>
       </c>
@@ -10475,7 +11041,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>131</v>
       </c>
@@ -10495,7 +11061,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>132</v>
       </c>
@@ -10515,7 +11081,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="4"/>
       <c r="B109" s="5"/>
       <c r="C109" s="12"/>
@@ -10523,27 +11089,384 @@
       <c r="F109" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.47244094488188981" right="0.39370078740157483" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="92" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="14" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="14" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="14" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="14" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="14" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>